<commit_message>
se sube version para que lo dscargue portales y use el de emisión Motor solamente
</commit_message>
<xml_diff>
--- a/DataSource/MaestroAltaPolizas.xlsx
+++ b/DataSource/MaestroAltaPolizas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\DataSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747455C9-63B1-4BD3-B7CB-0B77E5E9F6D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F1A7A6-5A2B-46F2-B743-CAF7BFEDDDB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="548">
   <si>
     <t>Ambiente</t>
   </si>
@@ -1277,18 +1277,6 @@
     <t>ZAZ123STA019</t>
   </si>
   <si>
-    <t>ZAZ123SET162</t>
-  </si>
-  <si>
-    <t>ZAZ123SET163</t>
-  </si>
-  <si>
-    <t>ZAZ123SET164</t>
-  </si>
-  <si>
-    <t>ZAZ123SET165</t>
-  </si>
-  <si>
     <t>NumeroDocumento</t>
   </si>
   <si>
@@ -1415,18 +1403,6 @@
     <t>ZAZ123SET206</t>
   </si>
   <si>
-    <t>ZAZ123SET211</t>
-  </si>
-  <si>
-    <t>ZAZ123SET212</t>
-  </si>
-  <si>
-    <t>ZAZ123SET213</t>
-  </si>
-  <si>
-    <t>ZAZ123SET214</t>
-  </si>
-  <si>
     <t>ZAZ123SET215</t>
   </si>
   <si>
@@ -1517,22 +1493,193 @@
     <t>ZAZ123FLT001</t>
   </si>
   <si>
-    <t>SME002</t>
-  </si>
-  <si>
-    <t>ABC12SME002</t>
-  </si>
-  <si>
-    <t>ZAZ12SME002</t>
-  </si>
-  <si>
-    <t>SME003</t>
-  </si>
-  <si>
-    <t>ABC12SME003</t>
-  </si>
-  <si>
-    <t>ZAZ12SME003</t>
+    <t>AON002</t>
+  </si>
+  <si>
+    <t>AON001</t>
+  </si>
+  <si>
+    <t>ABC12AON001</t>
+  </si>
+  <si>
+    <t>ZAZ12AON001</t>
+  </si>
+  <si>
+    <t>AON003</t>
+  </si>
+  <si>
+    <t>AON004</t>
+  </si>
+  <si>
+    <t>AON005</t>
+  </si>
+  <si>
+    <t>AON006</t>
+  </si>
+  <si>
+    <t>AON007</t>
+  </si>
+  <si>
+    <t>AON008</t>
+  </si>
+  <si>
+    <t>AON009</t>
+  </si>
+  <si>
+    <t>AON010</t>
+  </si>
+  <si>
+    <t>ABC12AON002</t>
+  </si>
+  <si>
+    <t>ABC12AON003</t>
+  </si>
+  <si>
+    <t>ABC12AON004</t>
+  </si>
+  <si>
+    <t>ABC12AON005</t>
+  </si>
+  <si>
+    <t>ABC12AON006</t>
+  </si>
+  <si>
+    <t>ABC12AON007</t>
+  </si>
+  <si>
+    <t>ABC12AON008</t>
+  </si>
+  <si>
+    <t>ABC12AON009</t>
+  </si>
+  <si>
+    <t>ABC12AON010</t>
+  </si>
+  <si>
+    <t>ZAZ12AON002</t>
+  </si>
+  <si>
+    <t>ZAZ12AON003</t>
+  </si>
+  <si>
+    <t>ZAZ12AON004</t>
+  </si>
+  <si>
+    <t>ZAZ12AON005</t>
+  </si>
+  <si>
+    <t>ZAZ12AON006</t>
+  </si>
+  <si>
+    <t>ZAZ12AON007</t>
+  </si>
+  <si>
+    <t>ZAZ12AON008</t>
+  </si>
+  <si>
+    <t>ZAZ12AON009</t>
+  </si>
+  <si>
+    <t>ZAZ12AON010</t>
+  </si>
+  <si>
+    <t>AON011</t>
+  </si>
+  <si>
+    <t>AON012</t>
+  </si>
+  <si>
+    <t>AON013</t>
+  </si>
+  <si>
+    <t>AON014</t>
+  </si>
+  <si>
+    <t>AON015</t>
+  </si>
+  <si>
+    <t>AON016</t>
+  </si>
+  <si>
+    <t>AON017</t>
+  </si>
+  <si>
+    <t>AON018</t>
+  </si>
+  <si>
+    <t>AON019</t>
+  </si>
+  <si>
+    <t>AON020</t>
+  </si>
+  <si>
+    <t>AON021</t>
+  </si>
+  <si>
+    <t>ABC12AON011</t>
+  </si>
+  <si>
+    <t>ABC12AON012</t>
+  </si>
+  <si>
+    <t>ABC12AON013</t>
+  </si>
+  <si>
+    <t>ABC12AON014</t>
+  </si>
+  <si>
+    <t>ABC12AON015</t>
+  </si>
+  <si>
+    <t>ABC12AON016</t>
+  </si>
+  <si>
+    <t>ABC12AON017</t>
+  </si>
+  <si>
+    <t>ABC12AON018</t>
+  </si>
+  <si>
+    <t>ABC12AON019</t>
+  </si>
+  <si>
+    <t>ABC12AON020</t>
+  </si>
+  <si>
+    <t>ABC12AON021</t>
+  </si>
+  <si>
+    <t>ZAZ12AON011</t>
+  </si>
+  <si>
+    <t>ZAZ12AON012</t>
+  </si>
+  <si>
+    <t>ZAZ12AON013</t>
+  </si>
+  <si>
+    <t>ZAZ12AON014</t>
+  </si>
+  <si>
+    <t>ZAZ12AON015</t>
+  </si>
+  <si>
+    <t>ZAZ12AON016</t>
+  </si>
+  <si>
+    <t>ZAZ12AON017</t>
+  </si>
+  <si>
+    <t>ZAZ12AON018</t>
+  </si>
+  <si>
+    <t>ZAZ12AON019</t>
+  </si>
+  <si>
+    <t>ZAZ12AON020</t>
+  </si>
+  <si>
+    <t>ZAZ12AON021</t>
   </si>
 </sst>
 </file>
@@ -1899,8 +2046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U350"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:T3"/>
+    <sheetView tabSelected="1" topLeftCell="I4" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11:T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2043,13 +2190,13 @@
         <v>32</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="U2" t="s">
         <v>33</v>
@@ -2108,13 +2255,13 @@
         <v>32</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>496</v>
+        <v>485</v>
       </c>
       <c r="S3" s="7" t="s">
         <v>497</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>498</v>
+        <v>506</v>
       </c>
       <c r="U3" t="s">
         <v>33</v>
@@ -2128,13 +2275,13 @@
       </c>
       <c r="L4" s="1"/>
       <c r="R4" s="7" t="s">
-        <v>63</v>
+        <v>489</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>292</v>
+        <v>498</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>390</v>
+        <v>507</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -2144,13 +2291,13 @@
       </c>
       <c r="L5" s="1"/>
       <c r="R5" s="7" t="s">
-        <v>64</v>
+        <v>490</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>293</v>
+        <v>499</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>391</v>
+        <v>508</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -2160,13 +2307,13 @@
       </c>
       <c r="L6" s="1"/>
       <c r="R6" s="7" t="s">
-        <v>65</v>
+        <v>491</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>294</v>
+        <v>500</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>392</v>
+        <v>509</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -2176,13 +2323,13 @@
       </c>
       <c r="L7" s="1"/>
       <c r="R7" s="7" t="s">
-        <v>66</v>
+        <v>492</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>295</v>
+        <v>501</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>393</v>
+        <v>510</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -2192,13 +2339,13 @@
       </c>
       <c r="L8" s="1"/>
       <c r="R8" s="7" t="s">
-        <v>127</v>
+        <v>493</v>
       </c>
       <c r="S8" s="7" t="s">
-        <v>356</v>
+        <v>502</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>459</v>
+        <v>511</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -2208,13 +2355,13 @@
       </c>
       <c r="L9" s="1"/>
       <c r="R9" s="7" t="s">
-        <v>68</v>
+        <v>494</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>297</v>
+        <v>503</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>395</v>
+        <v>512</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -2224,13 +2371,13 @@
       </c>
       <c r="L10" s="1"/>
       <c r="R10" s="7" t="s">
-        <v>69</v>
+        <v>495</v>
       </c>
       <c r="S10" s="7" t="s">
-        <v>298</v>
+        <v>504</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>396</v>
+        <v>513</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -2240,13 +2387,13 @@
       </c>
       <c r="L11" s="1"/>
       <c r="R11" s="7" t="s">
-        <v>70</v>
+        <v>496</v>
       </c>
       <c r="S11" s="7" t="s">
-        <v>299</v>
+        <v>505</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>397</v>
+        <v>514</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -2256,13 +2403,13 @@
       </c>
       <c r="L12" s="1"/>
       <c r="R12" s="7" t="s">
-        <v>128</v>
+        <v>515</v>
       </c>
       <c r="S12" s="7" t="s">
-        <v>357</v>
+        <v>526</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>460</v>
+        <v>537</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -2272,13 +2419,13 @@
       </c>
       <c r="L13" s="1"/>
       <c r="R13" s="7" t="s">
-        <v>72</v>
+        <v>516</v>
       </c>
       <c r="S13" s="7" t="s">
-        <v>301</v>
+        <v>527</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>399</v>
+        <v>538</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -2286,13 +2433,13 @@
         <v>4324449225</v>
       </c>
       <c r="R14" s="7" t="s">
-        <v>73</v>
+        <v>517</v>
       </c>
       <c r="S14" s="7" t="s">
-        <v>302</v>
+        <v>528</v>
       </c>
       <c r="T14" s="7" t="s">
-        <v>400</v>
+        <v>539</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -2302,13 +2449,13 @@
       </c>
       <c r="L15" s="1"/>
       <c r="R15" s="7" t="s">
-        <v>74</v>
+        <v>518</v>
       </c>
       <c r="S15" s="7" t="s">
-        <v>303</v>
+        <v>529</v>
       </c>
       <c r="T15" s="7" t="s">
-        <v>401</v>
+        <v>540</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -2318,13 +2465,13 @@
       </c>
       <c r="L16" s="1"/>
       <c r="R16" s="7" t="s">
-        <v>75</v>
+        <v>519</v>
       </c>
       <c r="S16" s="7" t="s">
-        <v>304</v>
+        <v>530</v>
       </c>
       <c r="T16" s="7" t="s">
-        <v>402</v>
+        <v>541</v>
       </c>
     </row>
     <row r="17" spans="2:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2334,70 +2481,70 @@
       </c>
       <c r="L17" s="6"/>
       <c r="R17" s="7" t="s">
-        <v>129</v>
+        <v>520</v>
       </c>
       <c r="S17" s="7" t="s">
-        <v>358</v>
+        <v>531</v>
       </c>
       <c r="T17" s="7" t="s">
-        <v>461</v>
+        <v>542</v>
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="L18" s="1"/>
       <c r="R18" s="7" t="s">
-        <v>130</v>
+        <v>521</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>359</v>
+        <v>532</v>
       </c>
       <c r="T18" s="7" t="s">
-        <v>462</v>
+        <v>543</v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="R19" s="7" t="s">
-        <v>78</v>
+        <v>522</v>
       </c>
       <c r="S19" s="7" t="s">
-        <v>307</v>
+        <v>533</v>
       </c>
       <c r="T19" s="7" t="s">
-        <v>413</v>
+        <v>544</v>
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="R20" s="7" t="s">
-        <v>79</v>
+        <v>523</v>
       </c>
       <c r="S20" s="7" t="s">
-        <v>308</v>
+        <v>534</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>414</v>
+        <v>545</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="R21" s="7" t="s">
-        <v>80</v>
+        <v>524</v>
       </c>
       <c r="S21" s="7" t="s">
-        <v>309</v>
+        <v>535</v>
       </c>
       <c r="T21" s="7" t="s">
-        <v>415</v>
+        <v>546</v>
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="R22" s="7" t="s">
-        <v>81</v>
+        <v>525</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>310</v>
+        <v>536</v>
       </c>
       <c r="T22" s="7" t="s">
-        <v>416</v>
+        <v>547</v>
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
@@ -2408,7 +2555,7 @@
         <v>360</v>
       </c>
       <c r="T23" s="7" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
@@ -2419,7 +2566,7 @@
         <v>312</v>
       </c>
       <c r="T24" s="7" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
@@ -2430,7 +2577,7 @@
         <v>313</v>
       </c>
       <c r="T25" s="7" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
@@ -2441,7 +2588,7 @@
         <v>314</v>
       </c>
       <c r="T26" s="7" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
@@ -2452,7 +2599,7 @@
         <v>315</v>
       </c>
       <c r="T27" s="7" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
@@ -2463,7 +2610,7 @@
         <v>316</v>
       </c>
       <c r="T28" s="7" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
@@ -2474,7 +2621,7 @@
         <v>317</v>
       </c>
       <c r="T29" s="7" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
@@ -2485,7 +2632,7 @@
         <v>318</v>
       </c>
       <c r="T30" s="7" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
@@ -2496,7 +2643,7 @@
         <v>319</v>
       </c>
       <c r="T31" s="7" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
@@ -2507,7 +2654,7 @@
         <v>320</v>
       </c>
       <c r="T32" s="7" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="33" spans="18:20" x14ac:dyDescent="0.25">
@@ -2518,7 +2665,7 @@
         <v>321</v>
       </c>
       <c r="T33" s="7" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="34" spans="18:20" x14ac:dyDescent="0.25">
@@ -2529,7 +2676,7 @@
         <v>322</v>
       </c>
       <c r="T34" s="7" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="35" spans="18:20" x14ac:dyDescent="0.25">
@@ -2540,7 +2687,7 @@
         <v>323</v>
       </c>
       <c r="T35" s="7" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="36" spans="18:20" x14ac:dyDescent="0.25">
@@ -2551,7 +2698,7 @@
         <v>324</v>
       </c>
       <c r="T36" s="7" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="37" spans="18:20" x14ac:dyDescent="0.25">
@@ -2562,7 +2709,7 @@
         <v>325</v>
       </c>
       <c r="T37" s="7" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="38" spans="18:20" x14ac:dyDescent="0.25">
@@ -2573,7 +2720,7 @@
         <v>326</v>
       </c>
       <c r="T38" s="7" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="39" spans="18:20" x14ac:dyDescent="0.25">
@@ -2584,7 +2731,7 @@
         <v>327</v>
       </c>
       <c r="T39" s="7" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="40" spans="18:20" x14ac:dyDescent="0.25">
@@ -2595,7 +2742,7 @@
         <v>328</v>
       </c>
       <c r="T40" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="41" spans="18:20" x14ac:dyDescent="0.25">
@@ -2606,7 +2753,7 @@
         <v>361</v>
       </c>
       <c r="T41" s="7" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
     </row>
     <row r="42" spans="18:20" x14ac:dyDescent="0.25">
@@ -2617,7 +2764,7 @@
         <v>330</v>
       </c>
       <c r="T42" s="7" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="43" spans="18:20" x14ac:dyDescent="0.25">
@@ -2628,7 +2775,7 @@
         <v>331</v>
       </c>
       <c r="T43" s="7" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="44" spans="18:20" x14ac:dyDescent="0.25">
@@ -2639,7 +2786,7 @@
         <v>332</v>
       </c>
       <c r="T44" s="7" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="45" spans="18:20" x14ac:dyDescent="0.25">
@@ -2650,7 +2797,7 @@
         <v>333</v>
       </c>
       <c r="T45" s="7" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="46" spans="18:20" x14ac:dyDescent="0.25">
@@ -2661,7 +2808,7 @@
         <v>334</v>
       </c>
       <c r="T46" s="7" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="47" spans="18:20" x14ac:dyDescent="0.25">
@@ -2672,7 +2819,7 @@
         <v>335</v>
       </c>
       <c r="T47" s="7" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="48" spans="18:20" x14ac:dyDescent="0.25">
@@ -2683,7 +2830,7 @@
         <v>336</v>
       </c>
       <c r="T48" s="7" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="49" spans="18:20" x14ac:dyDescent="0.25">
@@ -2694,7 +2841,7 @@
         <v>337</v>
       </c>
       <c r="T49" s="7" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="50" spans="18:20" x14ac:dyDescent="0.25">
@@ -2705,7 +2852,7 @@
         <v>338</v>
       </c>
       <c r="T50" s="7" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="51" spans="18:20" x14ac:dyDescent="0.25">
@@ -2716,7 +2863,7 @@
         <v>339</v>
       </c>
       <c r="T51" s="7" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="52" spans="18:20" x14ac:dyDescent="0.25">
@@ -2727,7 +2874,7 @@
         <v>340</v>
       </c>
       <c r="T52" s="7" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="53" spans="18:20" x14ac:dyDescent="0.25">
@@ -2738,7 +2885,7 @@
         <v>341</v>
       </c>
       <c r="T53" s="7" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="54" spans="18:20" x14ac:dyDescent="0.25">
@@ -2749,7 +2896,7 @@
         <v>342</v>
       </c>
       <c r="T54" s="7" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="55" spans="18:20" x14ac:dyDescent="0.25">
@@ -2760,7 +2907,7 @@
         <v>343</v>
       </c>
       <c r="T55" s="7" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="56" spans="18:20" x14ac:dyDescent="0.25">
@@ -2771,7 +2918,7 @@
         <v>344</v>
       </c>
       <c r="T56" s="7" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="57" spans="18:20" x14ac:dyDescent="0.25">
@@ -2782,7 +2929,7 @@
         <v>345</v>
       </c>
       <c r="T57" s="7" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="58" spans="18:20" x14ac:dyDescent="0.25">
@@ -2793,7 +2940,7 @@
         <v>346</v>
       </c>
       <c r="T58" s="7" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="59" spans="18:20" x14ac:dyDescent="0.25">
@@ -2804,7 +2951,7 @@
         <v>347</v>
       </c>
       <c r="T59" s="7" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="60" spans="18:20" x14ac:dyDescent="0.25">
@@ -2815,7 +2962,7 @@
         <v>348</v>
       </c>
       <c r="T60" s="7" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="61" spans="18:20" x14ac:dyDescent="0.25">
@@ -2826,7 +2973,7 @@
         <v>349</v>
       </c>
       <c r="T61" s="7" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="62" spans="18:20" x14ac:dyDescent="0.25">
@@ -2837,7 +2984,7 @@
         <v>350</v>
       </c>
       <c r="T62" s="7" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="63" spans="18:20" x14ac:dyDescent="0.25">
@@ -2848,7 +2995,7 @@
         <v>351</v>
       </c>
       <c r="T63" s="7" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="64" spans="18:20" x14ac:dyDescent="0.25">
@@ -2859,7 +3006,7 @@
         <v>362</v>
       </c>
       <c r="T64" s="7" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="65" spans="18:20" x14ac:dyDescent="0.25">
@@ -2870,7 +3017,7 @@
         <v>363</v>
       </c>
       <c r="T65" s="7" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
     </row>
     <row r="66" spans="18:20" x14ac:dyDescent="0.25">
@@ -2878,10 +3025,10 @@
         <v>135</v>
       </c>
       <c r="S66" s="7" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="T66" s="7" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
     <row r="67" spans="18:20" x14ac:dyDescent="0.25">
@@ -2889,10 +3036,10 @@
         <v>136</v>
       </c>
       <c r="S67" s="7" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="T67" s="7" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
     </row>
     <row r="68" spans="18:20" x14ac:dyDescent="0.25">
@@ -4793,79 +4940,79 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="B5" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="C5" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="B6" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="C6" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="B7" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="C7" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>470</v>
+      </c>
+      <c r="B8" t="s">
+        <v>474</v>
+      </c>
+      <c r="C8" t="s">
         <v>478</v>
-      </c>
-      <c r="B8" t="s">
-        <v>482</v>
-      </c>
-      <c r="C8" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>471</v>
+      </c>
+      <c r="B9" t="s">
+        <v>475</v>
+      </c>
+      <c r="C9" t="s">
         <v>479</v>
-      </c>
-      <c r="B9" t="s">
-        <v>483</v>
-      </c>
-      <c r="C9" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>472</v>
+      </c>
+      <c r="B10" t="s">
+        <v>476</v>
+      </c>
+      <c r="C10" t="s">
         <v>480</v>
-      </c>
-      <c r="B10" t="s">
-        <v>484</v>
-      </c>
-      <c r="C10" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>473</v>
+      </c>
+      <c r="B11" t="s">
+        <v>477</v>
+      </c>
+      <c r="C11" t="s">
         <v>481</v>
-      </c>
-      <c r="B11" t="s">
-        <v>485</v>
-      </c>
-      <c r="C11" t="s">
-        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -4897,13 +5044,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="B2" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="C2" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -4926,7 +5073,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se suben modificaciones hechas a los scripts de emision de flotas y nóminas
</commit_message>
<xml_diff>
--- a/DataSource/MaestroAltaPolizas.xlsx
+++ b/DataSource/MaestroAltaPolizas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\DataSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F1A7A6-5A2B-46F2-B743-CAF7BFEDDDB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5FA90E-D582-4DC6-8AB1-92FAE6788975}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="546">
   <si>
     <t>Ambiente</t>
   </si>
@@ -1493,193 +1493,187 @@
     <t>ZAZ123FLT001</t>
   </si>
   <si>
-    <t>AON002</t>
-  </si>
-  <si>
-    <t>AON001</t>
-  </si>
-  <si>
-    <t>ABC12AON001</t>
-  </si>
-  <si>
-    <t>ZAZ12AON001</t>
-  </si>
-  <si>
-    <t>AON003</t>
-  </si>
-  <si>
-    <t>AON004</t>
-  </si>
-  <si>
-    <t>AON005</t>
-  </si>
-  <si>
-    <t>AON006</t>
-  </si>
-  <si>
-    <t>AON007</t>
-  </si>
-  <si>
-    <t>AON008</t>
-  </si>
-  <si>
-    <t>AON009</t>
-  </si>
-  <si>
-    <t>AON010</t>
-  </si>
-  <si>
-    <t>ABC12AON002</t>
-  </si>
-  <si>
-    <t>ABC12AON003</t>
-  </si>
-  <si>
-    <t>ABC12AON004</t>
-  </si>
-  <si>
-    <t>ABC12AON005</t>
-  </si>
-  <si>
-    <t>ABC12AON006</t>
-  </si>
-  <si>
-    <t>ABC12AON007</t>
-  </si>
-  <si>
-    <t>ABC12AON008</t>
-  </si>
-  <si>
-    <t>ABC12AON009</t>
-  </si>
-  <si>
-    <t>ABC12AON010</t>
-  </si>
-  <si>
-    <t>ZAZ12AON002</t>
-  </si>
-  <si>
-    <t>ZAZ12AON003</t>
-  </si>
-  <si>
-    <t>ZAZ12AON004</t>
-  </si>
-  <si>
-    <t>ZAZ12AON005</t>
-  </si>
-  <si>
-    <t>ZAZ12AON006</t>
-  </si>
-  <si>
-    <t>ZAZ12AON007</t>
-  </si>
-  <si>
-    <t>ZAZ12AON008</t>
-  </si>
-  <si>
-    <t>ZAZ12AON009</t>
-  </si>
-  <si>
-    <t>ZAZ12AON010</t>
-  </si>
-  <si>
-    <t>AON011</t>
-  </si>
-  <si>
-    <t>AON012</t>
-  </si>
-  <si>
-    <t>AON013</t>
-  </si>
-  <si>
-    <t>AON014</t>
-  </si>
-  <si>
-    <t>AON015</t>
-  </si>
-  <si>
-    <t>AON016</t>
-  </si>
-  <si>
-    <t>AON017</t>
-  </si>
-  <si>
-    <t>AON018</t>
-  </si>
-  <si>
-    <t>AON019</t>
-  </si>
-  <si>
-    <t>AON020</t>
-  </si>
-  <si>
     <t>AON021</t>
   </si>
   <si>
-    <t>ABC12AON011</t>
-  </si>
-  <si>
-    <t>ABC12AON012</t>
-  </si>
-  <si>
-    <t>ABC12AON013</t>
-  </si>
-  <si>
-    <t>ABC12AON014</t>
-  </si>
-  <si>
-    <t>ABC12AON015</t>
-  </si>
-  <si>
-    <t>ABC12AON016</t>
-  </si>
-  <si>
-    <t>ABC12AON017</t>
-  </si>
-  <si>
-    <t>ABC12AON018</t>
-  </si>
-  <si>
-    <t>ABC12AON019</t>
-  </si>
-  <si>
-    <t>ABC12AON020</t>
-  </si>
-  <si>
     <t>ABC12AON021</t>
   </si>
   <si>
-    <t>ZAZ12AON011</t>
-  </si>
-  <si>
-    <t>ZAZ12AON012</t>
-  </si>
-  <si>
-    <t>ZAZ12AON013</t>
-  </si>
-  <si>
-    <t>ZAZ12AON014</t>
-  </si>
-  <si>
-    <t>ZAZ12AON015</t>
-  </si>
-  <si>
-    <t>ZAZ12AON016</t>
-  </si>
-  <si>
-    <t>ZAZ12AON017</t>
-  </si>
-  <si>
-    <t>ZAZ12AON018</t>
-  </si>
-  <si>
-    <t>ZAZ12AON019</t>
-  </si>
-  <si>
-    <t>ZAZ12AON020</t>
-  </si>
-  <si>
     <t>ZAZ12AON021</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON021</t>
+  </si>
+  <si>
+    <t>AON022</t>
+  </si>
+  <si>
+    <t>AON023</t>
+  </si>
+  <si>
+    <t>AON024</t>
+  </si>
+  <si>
+    <t>AON025</t>
+  </si>
+  <si>
+    <t>AON026</t>
+  </si>
+  <si>
+    <t>AON027</t>
+  </si>
+  <si>
+    <t>AON028</t>
+  </si>
+  <si>
+    <t>AON029</t>
+  </si>
+  <si>
+    <t>AON030</t>
+  </si>
+  <si>
+    <t>AON031</t>
+  </si>
+  <si>
+    <t>AON032</t>
+  </si>
+  <si>
+    <t>AON033</t>
+  </si>
+  <si>
+    <t>AON034</t>
+  </si>
+  <si>
+    <t>AON035</t>
+  </si>
+  <si>
+    <t>AON036</t>
+  </si>
+  <si>
+    <t>AON037</t>
+  </si>
+  <si>
+    <t>AON038</t>
+  </si>
+  <si>
+    <t>AON039</t>
+  </si>
+  <si>
+    <t>AON040</t>
+  </si>
+  <si>
+    <t>ABC12AON022</t>
+  </si>
+  <si>
+    <t>ABC12AON023</t>
+  </si>
+  <si>
+    <t>ABC12AON024</t>
+  </si>
+  <si>
+    <t>ABC12AON025</t>
+  </si>
+  <si>
+    <t>ABC12AON026</t>
+  </si>
+  <si>
+    <t>ABC12AON027</t>
+  </si>
+  <si>
+    <t>ABC12AON028</t>
+  </si>
+  <si>
+    <t>ABC12AON029</t>
+  </si>
+  <si>
+    <t>ABC12AON030</t>
+  </si>
+  <si>
+    <t>ABC12AON031</t>
+  </si>
+  <si>
+    <t>ABC12AON032</t>
+  </si>
+  <si>
+    <t>ABC12AON033</t>
+  </si>
+  <si>
+    <t>ABC12AON034</t>
+  </si>
+  <si>
+    <t>ABC12AON035</t>
+  </si>
+  <si>
+    <t>ABC12AON036</t>
+  </si>
+  <si>
+    <t>ABC12AON037</t>
+  </si>
+  <si>
+    <t>ABC12AON038</t>
+  </si>
+  <si>
+    <t>ABC12AON039</t>
+  </si>
+  <si>
+    <t>ABC12AON040</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON022</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON023</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON024</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON025</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON026</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON027</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON028</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON029</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON030</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON031</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON032</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON033</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON034</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON035</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON036</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON037</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON038</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON039</t>
+  </si>
+  <si>
+    <t>ZAZ12AAON040</t>
   </si>
 </sst>
 </file>
@@ -2046,8 +2040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U350"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I4" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11:T22"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,10 +2184,10 @@
         <v>32</v>
       </c>
       <c r="R2" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="S2" s="7" t="s">
         <v>486</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>487</v>
       </c>
       <c r="T2" s="7" t="s">
         <v>488</v>
@@ -2255,13 +2249,13 @@
         <v>32</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>497</v>
+        <v>508</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>506</v>
+        <v>527</v>
       </c>
       <c r="U3" t="s">
         <v>33</v>
@@ -2275,13 +2269,13 @@
       </c>
       <c r="L4" s="1"/>
       <c r="R4" s="7" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>498</v>
+        <v>509</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>507</v>
+        <v>528</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -2291,13 +2285,13 @@
       </c>
       <c r="L5" s="1"/>
       <c r="R5" s="7" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>499</v>
+        <v>510</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>508</v>
+        <v>529</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -2307,13 +2301,13 @@
       </c>
       <c r="L6" s="1"/>
       <c r="R6" s="7" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>500</v>
+        <v>511</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>509</v>
+        <v>530</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -2323,13 +2317,13 @@
       </c>
       <c r="L7" s="1"/>
       <c r="R7" s="7" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>501</v>
+        <v>512</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>510</v>
+        <v>531</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -2339,13 +2333,13 @@
       </c>
       <c r="L8" s="1"/>
       <c r="R8" s="7" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="S8" s="7" t="s">
-        <v>502</v>
+        <v>513</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>511</v>
+        <v>532</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -2355,13 +2349,13 @@
       </c>
       <c r="L9" s="1"/>
       <c r="R9" s="7" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>503</v>
+        <v>514</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>512</v>
+        <v>533</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -2371,13 +2365,13 @@
       </c>
       <c r="L10" s="1"/>
       <c r="R10" s="7" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="S10" s="7" t="s">
-        <v>504</v>
+        <v>515</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>513</v>
+        <v>534</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -2387,13 +2381,13 @@
       </c>
       <c r="L11" s="1"/>
       <c r="R11" s="7" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="S11" s="7" t="s">
-        <v>505</v>
+        <v>516</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>514</v>
+        <v>535</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -2403,13 +2397,13 @@
       </c>
       <c r="L12" s="1"/>
       <c r="R12" s="7" t="s">
-        <v>515</v>
+        <v>498</v>
       </c>
       <c r="S12" s="7" t="s">
-        <v>526</v>
+        <v>517</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -2419,13 +2413,13 @@
       </c>
       <c r="L13" s="1"/>
       <c r="R13" s="7" t="s">
-        <v>516</v>
+        <v>499</v>
       </c>
       <c r="S13" s="7" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -2433,13 +2427,13 @@
         <v>4324449225</v>
       </c>
       <c r="R14" s="7" t="s">
-        <v>517</v>
+        <v>500</v>
       </c>
       <c r="S14" s="7" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
       <c r="T14" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -2449,13 +2443,13 @@
       </c>
       <c r="L15" s="1"/>
       <c r="R15" s="7" t="s">
-        <v>518</v>
+        <v>501</v>
       </c>
       <c r="S15" s="7" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
       <c r="T15" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -2465,13 +2459,13 @@
       </c>
       <c r="L16" s="1"/>
       <c r="R16" s="7" t="s">
-        <v>519</v>
+        <v>502</v>
       </c>
       <c r="S16" s="7" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
       <c r="T16" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="17" spans="2:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2481,70 +2475,70 @@
       </c>
       <c r="L17" s="6"/>
       <c r="R17" s="7" t="s">
-        <v>520</v>
+        <v>503</v>
       </c>
       <c r="S17" s="7" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="T17" s="7" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="L18" s="1"/>
       <c r="R18" s="7" t="s">
-        <v>521</v>
+        <v>504</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="T18" s="7" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="R19" s="7" t="s">
-        <v>522</v>
+        <v>505</v>
       </c>
       <c r="S19" s="7" t="s">
-        <v>533</v>
+        <v>524</v>
       </c>
       <c r="T19" s="7" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="R20" s="7" t="s">
-        <v>523</v>
+        <v>506</v>
       </c>
       <c r="S20" s="7" t="s">
-        <v>534</v>
+        <v>525</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="R21" s="7" t="s">
-        <v>524</v>
+        <v>507</v>
       </c>
       <c r="S21" s="7" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
       <c r="T21" s="7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="R22" s="7" t="s">
-        <v>525</v>
+        <v>485</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>536</v>
+        <v>486</v>
       </c>
       <c r="T22" s="7" t="s">
-        <v>547</v>
+        <v>487</v>
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">

</xml_diff>